<commit_message>
First working version of the JPADPostProcessorExcel.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/JPADPostProcessorExcel/PostProcessorExcel_Output.xlsx
+++ b/JPADSandBox_v2/out/JPADPostProcessorExcel/PostProcessorExcel_Output.xlsx
@@ -82,8 +82,323 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="outer"/>
+          <c:w val="0.9"/>
+          <c:h val="0.95"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v> Y1</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet0!$B$5:$B$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet0!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v> Y2</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet0!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet0!$E$5:$E$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8.0"/>
+          <c:min val="1.0"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="770.0"/>
+          <c:min val="90.0"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="false"/>
+    </c:legend>
+    <c:plotVisOnly val="true"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="outer"/>
+          <c:w val="0.9"/>
+          <c:h val="0.95"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v> Y3</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12.0"/>
+          <c:min val="8.0"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1210.0"/>
+          <c:min val="810.0"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="true"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
@@ -161,11 +476,12 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -219,5 +535,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>